<commit_message>
unbalanced N solved for cached FFT
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>size</t>
   </si>
@@ -34,6 +34,18 @@
   </si>
   <si>
     <t>2D_FT_USING_1DFFT</t>
+  </si>
+  <si>
+    <t>cache_size</t>
+  </si>
+  <si>
+    <t>n=16777216</t>
+  </si>
+  <si>
+    <t>standart_FFT</t>
+  </si>
+  <si>
+    <t>cached_vectorized_FFT</t>
   </si>
 </sst>
 </file>
@@ -354,11 +366,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="200698880"/>
-        <c:axId val="200700672"/>
+        <c:axId val="200237824"/>
+        <c:axId val="200239360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="200698880"/>
+        <c:axId val="200237824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -368,7 +380,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200700672"/>
+        <c:crossAx val="200239360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -376,7 +388,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200700672"/>
+        <c:axId val="200239360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -387,7 +399,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200698880"/>
+        <c:crossAx val="200237824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -555,11 +567,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="200729728"/>
-        <c:axId val="200731264"/>
+        <c:axId val="200276608"/>
+        <c:axId val="241963392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="200729728"/>
+        <c:axId val="200276608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -569,7 +581,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200731264"/>
+        <c:crossAx val="241963392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -577,7 +589,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200731264"/>
+        <c:axId val="241963392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -588,7 +600,346 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200729728"/>
+        <c:crossAx val="200276608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$B$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cached_vectorized_FFT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист1!$A$33:$A$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>524288</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$33:$B$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>3.129</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9279999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6829999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.419</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4790000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.484</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.524</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3340000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.3540000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.3620000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.3780000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4780000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.5129999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.637</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$C$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>standart_FFT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист1!$A$33:$A$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>524288</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$C$33:$C$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="154854912"/>
+        <c:axId val="154856448"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="154854912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="154856448"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="154856448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="154854912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -667,6 +1018,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -962,10 +1343,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="Q34" sqref="Q34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,6 +1613,187 @@
       </c>
       <c r="C21">
         <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>3.129</v>
+      </c>
+      <c r="C33">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>64</v>
+      </c>
+      <c r="B34">
+        <v>2.9279999999999999</v>
+      </c>
+      <c r="C34">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>128</v>
+      </c>
+      <c r="B35">
+        <v>2.6829999999999998</v>
+      </c>
+      <c r="C35">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>256</v>
+      </c>
+      <c r="B36">
+        <v>2.6850000000000001</v>
+      </c>
+      <c r="C36">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>512</v>
+      </c>
+      <c r="B37">
+        <v>2.419</v>
+      </c>
+      <c r="C37">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1024</v>
+      </c>
+      <c r="B38">
+        <v>2.4790000000000001</v>
+      </c>
+      <c r="C38">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2048</v>
+      </c>
+      <c r="B39">
+        <v>2.484</v>
+      </c>
+      <c r="C39">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>4096</v>
+      </c>
+      <c r="B40">
+        <v>2.524</v>
+      </c>
+      <c r="C40">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>8192</v>
+      </c>
+      <c r="B41">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="C41">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>16384</v>
+      </c>
+      <c r="B42">
+        <v>2.3540000000000001</v>
+      </c>
+      <c r="C42">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>32768</v>
+      </c>
+      <c r="B43">
+        <v>2.3620000000000001</v>
+      </c>
+      <c r="C43">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>65536</v>
+      </c>
+      <c r="B44">
+        <v>2.3780000000000001</v>
+      </c>
+      <c r="C44">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>131072</v>
+      </c>
+      <c r="B45">
+        <v>2.4780000000000002</v>
+      </c>
+      <c r="C45">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>262144</v>
+      </c>
+      <c r="B46">
+        <v>2.5129999999999999</v>
+      </c>
+      <c r="C46">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>524288</v>
+      </c>
+      <c r="B47">
+        <v>2.637</v>
+      </c>
+      <c r="C47">
+        <v>2.2000000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first results of launching on the cluster
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" refMode="R1C1"/>
+  <calcPr calcId="145621" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>size</t>
   </si>
@@ -64,6 +64,42 @@
   </si>
   <si>
     <t>sincos pre-count</t>
+  </si>
+  <si>
+    <t>no buffer</t>
+  </si>
+  <si>
+    <t>no if</t>
+  </si>
+  <si>
+    <t>mkl</t>
+  </si>
+  <si>
+    <t>cache</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequental </t>
+  </si>
+  <si>
+    <t>1 thread</t>
+  </si>
+  <si>
+    <t>t/nlogn</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>my algorithm</t>
+  </si>
+  <si>
+    <t>threads</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>mkl e</t>
   </si>
 </sst>
 </file>
@@ -384,11 +420,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="204592256"/>
-        <c:axId val="204594176"/>
+        <c:axId val="219704320"/>
+        <c:axId val="219714688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="204592256"/>
+        <c:axId val="219704320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -418,7 +454,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="204594176"/>
+        <c:crossAx val="219714688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -426,7 +462,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="204594176"/>
+        <c:axId val="219714688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -457,7 +493,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="204592256"/>
+        <c:crossAx val="219704320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -625,11 +661,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="239419392"/>
-        <c:axId val="239421312"/>
+        <c:axId val="220669824"/>
+        <c:axId val="220680192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239419392"/>
+        <c:axId val="220669824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -659,7 +695,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239421312"/>
+        <c:crossAx val="220680192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -667,7 +703,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239421312"/>
+        <c:axId val="220680192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -698,7 +734,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239419392"/>
+        <c:crossAx val="220669824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1756,6 +1792,260 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$J$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>no buffer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист1!$A$33:$A$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>524288</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$J$33:$J$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.879</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.139</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.73099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.751</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.81399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.90700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.59799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.57699999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.57399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.56699999999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.69199999999999995</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.79800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.83499999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>no if</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист1!$A$33:$A$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>524288</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$K$33:$K$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.296</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.036</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.88600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0049999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.68700000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.84099999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.85299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.57399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.56699999999999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.56399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.68899999999999995</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.80700000000000005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.85499999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1766,11 +2056,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="239889792"/>
-        <c:axId val="239896064"/>
+        <c:axId val="220744704"/>
+        <c:axId val="220755072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239889792"/>
+        <c:axId val="220744704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1800,7 +2090,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239896064"/>
+        <c:crossAx val="220755072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1808,7 +2098,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239896064"/>
+        <c:axId val="220755072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1846,7 +2136,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239889792"/>
+        <c:crossAx val="220744704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1857,12 +2147,487 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.66450319908094557"/>
-          <c:y val="4.5422800410818219E-2"/>
+          <c:x val="0.67089297543877302"/>
+          <c:y val="5.7017003309368937E-2"/>
           <c:w val="0.32697709910861783"/>
           <c:h val="0.88596599338126214"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Асимптотика </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист1!$B$66:$B$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33554432</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>67108864</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>134217728</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>268435456</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$D$66:$D$74</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6.1378955841064453</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.4991769336518788</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8487470800226387</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.2881968125053067</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.360304395357768</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.3311805725097656</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.6005092033973103</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.4929385273544868</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.1928437267030993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="219417984"/>
+        <c:axId val="238093440"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="219417984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>N</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="238093440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="238093440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>t/NlogN</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="219417984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Strong scaling efficiency</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$G$79</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>e</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$G$80:$G$95</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.99998692810457512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.65464869281045757</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.47383006535947714</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.37377614379084967</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.32617647058823529</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2902271241830065</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.27141339869281039</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.23756209150326799</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.23498366013071895</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.2266111111111111</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.21276307189542487</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.19985620915032679</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.19661274509803922</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.1836503267973856</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.18377124183006532</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.17000816993464055</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$H$79</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mkl e</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$H$80:$H$95</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1.0005121951219511</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.64362764227642277</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.45295121951219519</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.37464715447154473</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.30494715447154469</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26593739837398372</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.24738699186991872</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.23400325203252034</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.21357642276422767</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.19235528455284553</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.17838943089430895</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.16773495934959351</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.15817154471544714</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.15888861788617886</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.15218943089430895</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.15159105691056912</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="237988096"/>
+        <c:axId val="238023040"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="237988096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="238023040"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="238023040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="237988096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1941,16 +2706,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1964,6 +2729,104 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>599615</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>28196</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Рисунок 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8420100" y="9001125"/>
+          <a:ext cx="3676190" cy="3028571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Диаграмма 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2259,15 +3122,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:V95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="R66" sqref="R66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2476,7 +3341,7 @@
         <v>13.747</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -2487,7 +3352,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1024</v>
       </c>
@@ -2498,7 +3363,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4096</v>
       </c>
@@ -2509,7 +3374,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16384</v>
       </c>
@@ -2520,7 +3385,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>65536</v>
       </c>
@@ -2531,12 +3396,12 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -2564,8 +3429,14 @@
       <c r="I32" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>16</v>
+      </c>
+      <c r="K32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2593,8 +3464,14 @@
       <c r="I33">
         <v>0.223</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33">
+        <v>0.998</v>
+      </c>
+      <c r="K33">
+        <v>1.296</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>64</v>
       </c>
@@ -2622,8 +3499,14 @@
       <c r="I34">
         <v>0.188</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34">
+        <v>0.999</v>
+      </c>
+      <c r="K34">
+        <v>1.036</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>128</v>
       </c>
@@ -2651,8 +3534,14 @@
       <c r="I35">
         <v>0.22600000000000001</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35">
+        <v>0.879</v>
+      </c>
+      <c r="K35">
+        <v>0.88600000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>256</v>
       </c>
@@ -2680,8 +3569,14 @@
       <c r="I36">
         <v>0.22800000000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36">
+        <v>1.139</v>
+      </c>
+      <c r="K36">
+        <v>1.0049999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>512</v>
       </c>
@@ -2709,8 +3604,14 @@
       <c r="I37">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="K37">
+        <v>0.68700000000000006</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1024</v>
       </c>
@@ -2738,8 +3639,14 @@
       <c r="I38">
         <v>0.184</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38">
+        <v>0.751</v>
+      </c>
+      <c r="K38">
+        <v>0.84099999999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2048</v>
       </c>
@@ -2767,8 +3674,14 @@
       <c r="I39">
         <v>0.188</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="K39">
+        <v>0.85299999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4096</v>
       </c>
@@ -2796,8 +3709,14 @@
       <c r="I40">
         <v>0.188</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="K40">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>8192</v>
       </c>
@@ -2825,8 +3744,14 @@
       <c r="I41">
         <v>0.187</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="K41">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>16384</v>
       </c>
@@ -2854,8 +3779,14 @@
       <c r="I42">
         <v>0.186</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="K42">
+        <v>0.57399999999999995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>32768</v>
       </c>
@@ -2883,8 +3814,14 @@
       <c r="I43">
         <v>0.22900000000000001</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="K43">
+        <v>0.56699999999999995</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>65536</v>
       </c>
@@ -2912,8 +3849,14 @@
       <c r="I44">
         <v>0.20899999999999999</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="K44">
+        <v>0.56399999999999995</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>131072</v>
       </c>
@@ -2941,8 +3884,14 @@
       <c r="I45">
         <v>0.185</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="K45">
+        <v>0.68899999999999995</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>262144</v>
       </c>
@@ -2970,8 +3919,14 @@
       <c r="I46">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="K46">
+        <v>0.80700000000000005</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>524288</v>
       </c>
@@ -2999,8 +3954,1087 @@
       <c r="I47">
         <v>0.20399999999999999</v>
       </c>
+      <c r="J47">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="K47">
+        <v>0.85499999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>524288</v>
+      </c>
+      <c r="D51">
+        <v>1048576</v>
+      </c>
+      <c r="E51">
+        <v>2097152</v>
+      </c>
+      <c r="F51">
+        <v>4194304</v>
+      </c>
+      <c r="G51">
+        <v>8388608</v>
+      </c>
+      <c r="H51">
+        <v>16777216</v>
+      </c>
+      <c r="I51">
+        <v>33554432</v>
+      </c>
+      <c r="J51" s="1">
+        <v>67108864</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>1024</v>
+      </c>
+      <c r="C52">
+        <v>1.4E-2</v>
+      </c>
+      <c r="D52">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="E52">
+        <v>0.106</v>
+      </c>
+      <c r="F52">
+        <v>0.19</v>
+      </c>
+      <c r="G52">
+        <v>0.375</v>
+      </c>
+      <c r="H52">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="I52">
+        <v>1.641</v>
+      </c>
+      <c r="J52">
+        <v>3.706</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>2048</v>
+      </c>
+      <c r="C53">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D53">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="E53">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="F53">
+        <v>0.217</v>
+      </c>
+      <c r="G53">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="H53">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="I53">
+        <v>1.784</v>
+      </c>
+      <c r="J53">
+        <v>3.7120000000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>4096</v>
+      </c>
+      <c r="C54">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="D54">
+        <v>0.03</v>
+      </c>
+      <c r="E54">
+        <v>6.3E-2</v>
+      </c>
+      <c r="F54">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="G54">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="H54">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="I54">
+        <v>1.7749999999999999</v>
+      </c>
+      <c r="J54">
+        <v>3.698</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>8192</v>
+      </c>
+      <c r="C55">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="D55">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="E55">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="F55">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="G55">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="H55">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="I55">
+        <v>1.286</v>
+      </c>
+      <c r="J55">
+        <v>3.5150000000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>16384</v>
+      </c>
+      <c r="C56">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D56">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="E56">
+        <v>0.06</v>
+      </c>
+      <c r="F56">
+        <v>0.127</v>
+      </c>
+      <c r="G56">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H56">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="I56">
+        <v>1.2549999999999999</v>
+      </c>
+      <c r="J56">
+        <v>2.6669999999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>32768</v>
+      </c>
+      <c r="C57">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D57">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="E57">
+        <v>0.06</v>
+      </c>
+      <c r="F57">
+        <v>0.124</v>
+      </c>
+      <c r="G57">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="H57">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="I57">
+        <v>1.2310000000000001</v>
+      </c>
+      <c r="J57">
+        <v>2.625</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>65536</v>
+      </c>
+      <c r="C58">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D58">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="E58">
+        <v>6.2E-2</v>
+      </c>
+      <c r="F58">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="G58">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="H58">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="I58">
+        <v>1.2290000000000001</v>
+      </c>
+      <c r="J58">
+        <v>2.6379999999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>131072</v>
+      </c>
+      <c r="C59">
+        <v>2.4E-2</v>
+      </c>
+      <c r="D59">
+        <v>3.9E-2</v>
+      </c>
+      <c r="E59">
+        <v>0.08</v>
+      </c>
+      <c r="F59">
+        <v>0.161</v>
+      </c>
+      <c r="G59">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="H59">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="I59">
+        <v>1.4730000000000001</v>
+      </c>
+      <c r="J59">
+        <v>3.1150000000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>262144</v>
+      </c>
+      <c r="C60">
+        <v>2.7E-2</v>
+      </c>
+      <c r="D60">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="E60">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="F60">
+        <v>0.191</v>
+      </c>
+      <c r="G60">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="H60">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="I60">
+        <v>1.71</v>
+      </c>
+      <c r="J60">
+        <v>3.6269999999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>524288</v>
+      </c>
+      <c r="C61">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="D61">
+        <v>6.2E-2</v>
+      </c>
+      <c r="E61">
+        <v>0.115</v>
+      </c>
+      <c r="F61">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="G61">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="H61">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="I61">
+        <v>1.7909999999999999</v>
+      </c>
+      <c r="J61">
+        <v>3.7349999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="D62">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E62">
+        <v>2.3E-2</v>
+      </c>
+      <c r="F62">
+        <v>0.06</v>
+      </c>
+      <c r="G62">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="H62">
+        <v>0.188</v>
+      </c>
+      <c r="I62">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="J62" s="1">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" t="s">
+        <v>19</v>
+      </c>
+      <c r="D65" t="s">
+        <v>22</v>
+      </c>
+      <c r="E65" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>1048576</v>
+      </c>
+      <c r="C66">
+        <v>65536</v>
+      </c>
+      <c r="D66" s="1">
+        <f>E66/(B66*LOG(B66,2))*1000000000</f>
+        <v>6.1378955841064453</v>
+      </c>
+      <c r="E66" s="1">
+        <v>0.128721</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>2097152</v>
+      </c>
+      <c r="C67">
+        <v>65536</v>
+      </c>
+      <c r="D67" s="1">
+        <f>E67/(B67*LOG(B67,2))*1000000000</f>
+        <v>6.4991769336518788</v>
+      </c>
+      <c r="E67" s="1">
+        <v>0.28622500000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>4194304</v>
+      </c>
+      <c r="C68">
+        <v>65536</v>
+      </c>
+      <c r="D68" s="1">
+        <f>E68/(B68*LOG(B68,2))*1000000000</f>
+        <v>6.8487470800226387</v>
+      </c>
+      <c r="E68" s="1">
+        <v>0.63196600000000003</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>8388608</v>
+      </c>
+      <c r="C69">
+        <v>65536</v>
+      </c>
+      <c r="D69" s="1">
+        <f>E69/(B69*LOG(B69,2))*1000000000</f>
+        <v>7.2881968125053067</v>
+      </c>
+      <c r="E69" s="1">
+        <v>1.4061699999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>16777216</v>
+      </c>
+      <c r="C70">
+        <v>65536</v>
+      </c>
+      <c r="D70" s="1">
+        <f>E70/(B70*LOG(B70,2))*1000000000</f>
+        <v>7.360304395357768</v>
+      </c>
+      <c r="E70" s="1">
+        <v>2.9636499999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>33554432</v>
+      </c>
+      <c r="C71">
+        <v>65536</v>
+      </c>
+      <c r="D71" s="1">
+        <f>E71/(B71*LOG(B71,2))*1000000000</f>
+        <v>7.3311805725097656</v>
+      </c>
+      <c r="E71" s="1">
+        <v>6.1498400000000002</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>67108864</v>
+      </c>
+      <c r="C72">
+        <v>65536</v>
+      </c>
+      <c r="D72" s="1">
+        <f>E72/(B72*LOG(B72,2))*1000000000</f>
+        <v>7.6005092033973103</v>
+      </c>
+      <c r="E72" s="1">
+        <v>13.2616</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>134217728</v>
+      </c>
+      <c r="C73">
+        <v>65536</v>
+      </c>
+      <c r="D73" s="1">
+        <f>E73/(B73*LOG(B73,2))*1000000000</f>
+        <v>7.4929385273544868</v>
+      </c>
+      <c r="E73" s="1">
+        <v>27.153500000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>268435456</v>
+      </c>
+      <c r="C74">
+        <v>65536</v>
+      </c>
+      <c r="D74" s="1">
+        <f>E74/(B74*LOG(B74,2))*1000000000</f>
+        <v>7.1928437267030993</v>
+      </c>
+      <c r="E74" s="1">
+        <v>54.062800000000003</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>0</v>
+      </c>
+      <c r="C79" t="s">
+        <v>19</v>
+      </c>
+      <c r="D79" t="s">
+        <v>25</v>
+      </c>
+      <c r="E79" t="s">
+        <v>24</v>
+      </c>
+      <c r="F79" t="s">
+        <v>18</v>
+      </c>
+      <c r="G79" t="s">
+        <v>26</v>
+      </c>
+      <c r="H79" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>33554432</v>
+      </c>
+      <c r="C80">
+        <v>65536</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="E80" s="1">
+        <v>6.1199199999999996</v>
+      </c>
+      <c r="F80" s="1">
+        <v>1.2306299999999999</v>
+      </c>
+      <c r="G80" s="1">
+        <f>(E80/(6.12/D80))/D80</f>
+        <v>0.99998692810457512</v>
+      </c>
+      <c r="H80" s="1">
+        <f>(F80/(1.23/D80))/D80</f>
+        <v>1.0005121951219511</v>
+      </c>
+    </row>
+    <row r="81" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>33554432</v>
+      </c>
+      <c r="C81">
+        <v>65536</v>
+      </c>
+      <c r="D81">
+        <v>2</v>
+      </c>
+      <c r="E81" s="1">
+        <v>4.0064500000000001</v>
+      </c>
+      <c r="F81" s="1">
+        <v>0.79166199999999998</v>
+      </c>
+      <c r="G81" s="1">
+        <f t="shared" ref="G81:G95" si="0">(E81/(6.12/D81))/D81</f>
+        <v>0.65464869281045757</v>
+      </c>
+      <c r="H81" s="1">
+        <f t="shared" ref="H81:H95" si="1">(F81/(1.23/D81))/D81</f>
+        <v>0.64362764227642277</v>
+      </c>
+      <c r="R81" t="s">
+        <v>0</v>
+      </c>
+      <c r="S81" t="s">
+        <v>19</v>
+      </c>
+      <c r="T81" t="s">
+        <v>20</v>
+      </c>
+      <c r="U81" t="s">
+        <v>21</v>
+      </c>
+      <c r="V81" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>33554432</v>
+      </c>
+      <c r="C82">
+        <v>65536</v>
+      </c>
+      <c r="D82">
+        <v>3</v>
+      </c>
+      <c r="E82" s="1">
+        <v>2.8998400000000002</v>
+      </c>
+      <c r="F82" s="1">
+        <v>0.55713000000000001</v>
+      </c>
+      <c r="G82" s="1">
+        <f t="shared" si="0"/>
+        <v>0.47383006535947714</v>
+      </c>
+      <c r="H82" s="1">
+        <f t="shared" si="1"/>
+        <v>0.45295121951219519</v>
+      </c>
+      <c r="R82">
+        <v>33554432</v>
+      </c>
+      <c r="S82">
+        <v>32768</v>
+      </c>
+      <c r="T82" s="1">
+        <v>6.3910900000000002</v>
+      </c>
+      <c r="U82" s="1">
+        <v>6.2534200000000002</v>
+      </c>
+      <c r="V82" s="1">
+        <v>1.22488</v>
+      </c>
+    </row>
+    <row r="83" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>33554432</v>
+      </c>
+      <c r="C83">
+        <v>65536</v>
+      </c>
+      <c r="D83">
+        <v>4</v>
+      </c>
+      <c r="E83" s="1">
+        <v>2.2875100000000002</v>
+      </c>
+      <c r="F83" s="1">
+        <v>0.460816</v>
+      </c>
+      <c r="G83" s="1">
+        <f t="shared" si="0"/>
+        <v>0.37377614379084967</v>
+      </c>
+      <c r="H83" s="1">
+        <f t="shared" si="1"/>
+        <v>0.37464715447154473</v>
+      </c>
+      <c r="R83">
+        <v>33554432</v>
+      </c>
+      <c r="S83">
+        <v>65536</v>
+      </c>
+      <c r="T83" s="1">
+        <v>6.1840599999999997</v>
+      </c>
+      <c r="U83" s="1">
+        <v>6.1080699999999997</v>
+      </c>
+      <c r="V83" s="1">
+        <v>1.3779300000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>33554432</v>
+      </c>
+      <c r="C84">
+        <v>65536</v>
+      </c>
+      <c r="D84">
+        <v>5</v>
+      </c>
+      <c r="E84" s="1">
+        <v>1.9962</v>
+      </c>
+      <c r="F84" s="1">
+        <v>0.375085</v>
+      </c>
+      <c r="G84" s="1">
+        <f t="shared" si="0"/>
+        <v>0.32617647058823529</v>
+      </c>
+      <c r="H84" s="1">
+        <f t="shared" si="1"/>
+        <v>0.30494715447154469</v>
+      </c>
+      <c r="R84">
+        <v>33554432</v>
+      </c>
+      <c r="S84">
+        <v>131072</v>
+      </c>
+      <c r="T84" s="1">
+        <v>6.0389099999999996</v>
+      </c>
+      <c r="U84" s="1">
+        <v>5.9727600000000001</v>
+      </c>
+      <c r="V84" s="1">
+        <v>1.5501400000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>33554432</v>
+      </c>
+      <c r="C85">
+        <v>65536</v>
+      </c>
+      <c r="D85">
+        <v>6</v>
+      </c>
+      <c r="E85" s="1">
+        <v>1.7761899999999999</v>
+      </c>
+      <c r="F85" s="1">
+        <v>0.32710299999999998</v>
+      </c>
+      <c r="G85" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2902271241830065</v>
+      </c>
+      <c r="H85" s="1">
+        <f t="shared" si="1"/>
+        <v>0.26593739837398372</v>
+      </c>
+    </row>
+    <row r="86" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>33554432</v>
+      </c>
+      <c r="C86">
+        <v>65536</v>
+      </c>
+      <c r="D86">
+        <v>7</v>
+      </c>
+      <c r="E86" s="1">
+        <v>1.6610499999999999</v>
+      </c>
+      <c r="F86" s="1">
+        <v>0.304286</v>
+      </c>
+      <c r="G86" s="1">
+        <f t="shared" si="0"/>
+        <v>0.27141339869281039</v>
+      </c>
+      <c r="H86" s="1">
+        <f t="shared" si="1"/>
+        <v>0.24738699186991872</v>
+      </c>
+    </row>
+    <row r="87" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>33554432</v>
+      </c>
+      <c r="C87">
+        <v>65536</v>
+      </c>
+      <c r="D87">
+        <v>8</v>
+      </c>
+      <c r="E87" s="1">
+        <v>1.4538800000000001</v>
+      </c>
+      <c r="F87" s="1">
+        <v>0.28782400000000002</v>
+      </c>
+      <c r="G87" s="1">
+        <f t="shared" si="0"/>
+        <v>0.23756209150326799</v>
+      </c>
+      <c r="H87" s="1">
+        <f t="shared" si="1"/>
+        <v>0.23400325203252034</v>
+      </c>
+    </row>
+    <row r="88" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>33554432</v>
+      </c>
+      <c r="C88">
+        <v>65536</v>
+      </c>
+      <c r="D88">
+        <v>9</v>
+      </c>
+      <c r="E88" s="1">
+        <v>1.4380999999999999</v>
+      </c>
+      <c r="F88" s="1">
+        <v>0.26269900000000002</v>
+      </c>
+      <c r="G88" s="1">
+        <f t="shared" si="0"/>
+        <v>0.23498366013071895</v>
+      </c>
+      <c r="H88" s="1">
+        <f t="shared" si="1"/>
+        <v>0.21357642276422767</v>
+      </c>
+    </row>
+    <row r="89" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>33554432</v>
+      </c>
+      <c r="C89">
+        <v>65536</v>
+      </c>
+      <c r="D89">
+        <v>10</v>
+      </c>
+      <c r="E89" s="1">
+        <v>1.38686</v>
+      </c>
+      <c r="F89" s="1">
+        <v>0.236597</v>
+      </c>
+      <c r="G89" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2266111111111111</v>
+      </c>
+      <c r="H89" s="1">
+        <f t="shared" si="1"/>
+        <v>0.19235528455284553</v>
+      </c>
+    </row>
+    <row r="90" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>33554432</v>
+      </c>
+      <c r="C90">
+        <v>65536</v>
+      </c>
+      <c r="D90">
+        <v>11</v>
+      </c>
+      <c r="E90" s="1">
+        <v>1.3021100000000001</v>
+      </c>
+      <c r="F90" s="1">
+        <v>0.219419</v>
+      </c>
+      <c r="G90" s="1">
+        <f t="shared" si="0"/>
+        <v>0.21276307189542487</v>
+      </c>
+      <c r="H90" s="1">
+        <f t="shared" si="1"/>
+        <v>0.17838943089430895</v>
+      </c>
+    </row>
+    <row r="91" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>33554432</v>
+      </c>
+      <c r="C91">
+        <v>65536</v>
+      </c>
+      <c r="D91">
+        <v>12</v>
+      </c>
+      <c r="E91" s="1">
+        <v>1.22312</v>
+      </c>
+      <c r="F91" s="1">
+        <v>0.206314</v>
+      </c>
+      <c r="G91" s="1">
+        <f t="shared" si="0"/>
+        <v>0.19985620915032679</v>
+      </c>
+      <c r="H91" s="1">
+        <f t="shared" si="1"/>
+        <v>0.16773495934959351</v>
+      </c>
+    </row>
+    <row r="92" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>33554432</v>
+      </c>
+      <c r="C92">
+        <v>65536</v>
+      </c>
+      <c r="D92">
+        <v>13</v>
+      </c>
+      <c r="E92" s="1">
+        <v>1.2032700000000001</v>
+      </c>
+      <c r="F92" s="1">
+        <v>0.194551</v>
+      </c>
+      <c r="G92" s="1">
+        <f t="shared" si="0"/>
+        <v>0.19661274509803922</v>
+      </c>
+      <c r="H92" s="1">
+        <f t="shared" si="1"/>
+        <v>0.15817154471544714</v>
+      </c>
+    </row>
+    <row r="93" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>33554432</v>
+      </c>
+      <c r="C93">
+        <v>65536</v>
+      </c>
+      <c r="D93">
+        <v>14</v>
+      </c>
+      <c r="E93" s="1">
+        <v>1.1239399999999999</v>
+      </c>
+      <c r="F93" s="1">
+        <v>0.195433</v>
+      </c>
+      <c r="G93" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1836503267973856</v>
+      </c>
+      <c r="H93" s="1">
+        <f t="shared" si="1"/>
+        <v>0.15888861788617886</v>
+      </c>
+    </row>
+    <row r="94" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>33554432</v>
+      </c>
+      <c r="C94">
+        <v>65536</v>
+      </c>
+      <c r="D94">
+        <v>15</v>
+      </c>
+      <c r="E94" s="1">
+        <v>1.1246799999999999</v>
+      </c>
+      <c r="F94" s="1">
+        <v>0.187193</v>
+      </c>
+      <c r="G94" s="1">
+        <f t="shared" si="0"/>
+        <v>0.18377124183006532</v>
+      </c>
+      <c r="H94" s="1">
+        <f t="shared" si="1"/>
+        <v>0.15218943089430895</v>
+      </c>
+    </row>
+    <row r="95" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>33554432</v>
+      </c>
+      <c r="C95">
+        <v>65536</v>
+      </c>
+      <c r="D95">
+        <v>16</v>
+      </c>
+      <c r="E95" s="1">
+        <v>1.0404500000000001</v>
+      </c>
+      <c r="F95" s="1">
+        <v>0.18645700000000001</v>
+      </c>
+      <c r="G95" s="1">
+        <f t="shared" si="0"/>
+        <v>0.17000816993464055</v>
+      </c>
+      <c r="H95" s="1">
+        <f t="shared" si="1"/>
+        <v>0.15159105691056912</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F52:F61">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G52:G61">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H52:H61">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I52:I61">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J52:J61">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E52:E61">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D52:D61">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52:C61">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>